<commit_message>
show learnin category icon by image path
</commit_message>
<xml_diff>
--- a/EnglishApp/Assets.xcassets/TestLearningCategories.dataset/LearningCategories.xlsx
+++ b/EnglishApp/Assets.xcassets/TestLearningCategories.dataset/LearningCategories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Projects/Xcode/EnglishApp/EnglishApp/EnglishApp/Assets.xcassets/TestLearningCategories.dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569BE22A-128D-5747-97A6-569AD52BAED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0081428-9A4B-414E-9072-02360DD65858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -52,18 +51,12 @@
     <t>Яблоко</t>
   </si>
   <si>
-    <t>CategoryIcon0</t>
-  </si>
-  <si>
     <t>ТОП 100</t>
   </si>
   <si>
     <t>для начинающих</t>
   </si>
   <si>
-    <t>Имя файла иконки</t>
-  </si>
-  <si>
     <t>Заголовок</t>
   </si>
   <si>
@@ -74,16 +67,30 @@
   </si>
   <si>
     <t>#98E27F</t>
+  </si>
+  <si>
+    <t>Путь к картинке иконки</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Square_Flag_of_the_United_Kingdom.svg/1024px-Square_Flag_of_the_United_Kingdom.svg.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,14 +113,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,12 +439,12 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
@@ -448,16 +458,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -467,17 +477,17 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -489,6 +499,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{876EB980-87D4-7C4D-B003-891E2475DBA7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>